<commit_message>
Modify the script of 0-2 war
1. Modify the flow of script of 0-2 war
2. Increase the timeout of wait_image_gone in image.py
3. Add and update some images
</commit_message>
<xml_diff>
--- a/battle/wars/0-2/0-2.xlsx
+++ b/battle/wars/0-2/0-2.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,22 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>374, 270</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>400, 110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>400, 268</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>504, 116</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>blank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,10 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>504, 268</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>392, 194</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -244,6 +224,14 @@
   </si>
   <si>
     <t>wait_image_gone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400, 422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>502, 266</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -661,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -671,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -706,11 +694,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -720,7 +708,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -728,7 +716,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
@@ -738,213 +726,223 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3">
-        <v>10</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D30" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>